<commit_message>
hw - ledboard, compensation
</commit_message>
<xml_diff>
--- a/hw/ledBoard/FB_devider.xlsx
+++ b/hw/ledBoard/FB_devider.xlsx
@@ -107,11 +107,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -662,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.69999999999999996</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -672,8 +671,8 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
+      <c r="B3" s="1">
+        <v>8.5589999999999993</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -683,7 +682,7 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>12</v>
       </c>
       <c r="C4" t="s">
@@ -718,49 +717,49 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f>(B4-C10)/D10</f>
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="C9">
         <f>B9*D9</f>
-        <v>3.4461538461538463</v>
-      </c>
-      <c r="D9" s="5">
+        <v>7.9589999999999996</v>
+      </c>
+      <c r="D9" s="4">
         <f>D10-D11</f>
-        <v>0.024615384615384615</v>
+        <v>0.041889473684210525</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>10</v>
       </c>
-      <c r="C10">
-        <v>0.80000000000000004</v>
-      </c>
-      <c r="D10" s="5">
-        <f>C10/B10</f>
-        <v>0.080000000000000002</v>
+      <c r="C10" s="1">
+        <v>0.59999999999999998</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" ref="D10:D11" si="0">C10/B10</f>
+        <v>0.059999999999999998</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4">
-        <f>(G1-B2-B3)/D10</f>
-        <v>32.499999999999993</v>
+      <c r="B11" s="3">
+        <f>(G1-B2-C10)/(D10-(B3-C10)/(B9))</f>
+        <v>126.99796570764312</v>
       </c>
       <c r="C11">
         <f>MAX(B1-B2-C10,0)</f>
-        <v>1.7999999999999996</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D11">
-        <f>C11/B11</f>
-        <v>0.055384615384615386</v>
+        <f t="shared" si="0"/>
+        <v>0.018110526315789473</v>
       </c>
     </row>
     <row r="12" ht="14.25"/>
@@ -768,9 +767,9 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f>C9+C10</f>
-        <v>4.2461538461538462</v>
+        <v>8.5589999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hw - led board redesign
</commit_message>
<xml_diff>
--- a/hw/ledBoard/FB_devider.xlsx
+++ b/hw/ledBoard/FB_devider.xlsx
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>3.2999999999999998</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.40000000000000002</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -672,7 +672,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>8.5589999999999993</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -719,15 +719,15 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-C10)/D10</f>
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="C9">
         <f>B9*D9</f>
-        <v>7.9589999999999996</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="D9" s="4">
         <f>D10-D11</f>
-        <v>0.041889473684210525</v>
+        <v>0.080000000000000002</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -738,11 +738,11 @@
         <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>0.59999999999999998</v>
+        <v>0.80000000000000004</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" ref="D10:D11" si="0">C10/B10</f>
-        <v>0.059999999999999998</v>
+        <v>0.080000000000000002</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -751,15 +751,15 @@
       </c>
       <c r="B11" s="3">
         <f>(G1-B2-C10)/(D10-(B3-C10)/(B9))</f>
-        <v>126.99796570764312</v>
+        <v>100.33333333333327</v>
       </c>
       <c r="C11">
         <f>MAX(B1-B2-C10,0)</f>
-        <v>2.2999999999999998</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.018110526315789473</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="14.25"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="C13" s="6">
         <f>C9+C10</f>
-        <v>8.5589999999999993</v>
+        <v>12.000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>